<commit_message>
Demo on Dynamic Xpath
</commit_message>
<xml_diff>
--- a/SeleniumFramework/src/test/resources/config/testdata.xlsx
+++ b/SeleniumFramework/src/test/resources/config/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagaru\RestAssured\SeleniumFramework\src\test\resources\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagaru\git\SeleniumJavaFramework\SeleniumFramework\src\test\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEA904D-530D-4342-94A7-1005BBD2A49B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F6EB35-4FC9-4CFA-803D-8DFBA80CE64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20670" windowHeight="10080" activeTab="2" xr2:uid="{E2B3C879-1491-4308-9F07-02FD97CCA896}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>username</t>
   </si>
@@ -143,6 +143,27 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>Amazon Demo Test</t>
+  </si>
+  <si>
+    <t>menuOption</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+  <si>
+    <t>amazonDemoTest</t>
+  </si>
+  <si>
+    <t>subMenuOption</t>
+  </si>
+  <si>
+    <t>Mobiles, Computers</t>
   </si>
 </sst>
 </file>
@@ -572,15 +593,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B2D761-D33F-4352-8CB5-1CC2AB05F920}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -609,7 +630,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>25</v>
@@ -632,6 +653,23 @@
         <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -642,22 +680,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA94F2BA-0464-49C4-82DE-65FDE038AEBF}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -676,8 +716,14 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -696,8 +742,14 @@
       <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -716,8 +768,14 @@
       <c r="F3" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -736,8 +794,14 @@
       <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -756,86 +820,38 @@
       <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>